<commit_message>
template generated appropriatelly, stream refactured, test coverage
</commit_message>
<xml_diff>
--- a/simpleTS/simpleTest.xlsx
+++ b/simpleTS/simpleTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>Test for tranlation to js file</t>
   </si>
@@ -28,26 +28,23 @@
     <t>BankAustria</t>
   </si>
   <si>
-    <t>"credentials": {  "countryCode": "280",
+    <t>getAccounts</t>
+  </si>
+  <si>
+    <t>{"credentials": {  "countryCode": "280",
     "custID": "",
     "custID2": "",
     "hbciVersion": "0",
     "language": 1,
     "url": "bawagPSK.js",
     "userID": "64769092",
-    "pin": "38567" }</t>
-  </si>
-  <si>
-    <t>"pin": "38567"</t>
-  </si>
-  <si>
-    <t>"tasks": [ "getAccounts"  ]</t>
+    "pin": "38567" }}</t>
+  </si>
+  <si>
+    <t>||</t>
   </si>
   <si>
     <t>|</t>
-  </si>
-  <si>
-    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -159,45 +156,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="106.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="184.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="184.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f aca="false">E3</f>
+        <v>{"credentials": {  "countryCode": "280",
+    "custID": "",
+    "custID2": "",
+    "hbciVersion": "0",
+    "language": 1,
+    "url": "bawagPSK.js",
+    "userID": "64769092",
+    "pin": "38567" }}</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="184.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f aca="false">C4</f>
+        <v>{"credentials": {  "countryCode": "280",
+    "custID": "",
+    "custID2": "",
+    "hbciVersion": "0",
+    "language": 1,
+    "url": "bawagPSK.js",
+    "userID": "64769092",
+    "pin": "38567" }}</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generation with references + addition to conventions
</commit_message>
<xml_diff>
--- a/simpleTS/simpleTest.xlsx
+++ b/simpleTS/simpleTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Test for tranlation to js file</t>
   </si>
@@ -31,14 +31,20 @@
     <t>getAccounts</t>
   </si>
   <si>
-    <t>{"credentials": {  "countryCode": "280",
+    <t> {  "countryCode": "280",
     "custID": "",
     "custID2": "",
     "hbciVersion": "0",
     "language": 1,
     "url": "bawagPSK.js",
     "userID": "64769092",
-    "pin": "38567" }}</t>
+    "pin": "38567" }</t>
+  </si>
+  <si>
+    <t>“38567”</t>
+  </si>
+  <si>
+    <t>”12345”</t>
   </si>
   <si>
     <t>||</t>
@@ -156,10 +162,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -189,10 +195,16 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -204,20 +216,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f aca="false">E3</f>
-        <v>{"credentials": {  "countryCode": "280",
+        <f aca="false">C3</f>
+        <v> {  "countryCode": "280",
     "custID": "",
     "custID2": "",
     "hbciVersion": "0",
     "language": 1,
     "url": "bawagPSK.js",
     "userID": "64769092",
-    "pin": "38567" }}</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
+    "pin": "38567" }</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -230,19 +244,23 @@
       </c>
       <c r="C5" s="2" t="str">
         <f aca="false">C4</f>
-        <v>{"credentials": {  "countryCode": "280",
+        <v> {  "countryCode": "280",
     "custID": "",
     "custID2": "",
     "hbciVersion": "0",
     "language": 1,
     "url": "bawagPSK.js",
     "userID": "64769092",
-    "pin": "38567" }}</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    "pin": "38567" }</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reference scheme excluded, styles to scheme added
</commit_message>
<xml_diff>
--- a/simpleTS/simpleTest.xlsx
+++ b/simpleTS/simpleTest.xlsx
@@ -60,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -89,13 +89,38 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CC00"/>
+        <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,13 +157,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -154,6 +195,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF66CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -165,7 +266,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -195,16 +296,16 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -215,9 +316,9 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="str">
+      <c r="C4" s="5" t="str">
         <f aca="false">C3</f>
-        <v> {  "countryCode": "280",
+        <v>{  "countryCode": "280",
     "custID": "",
     "custID2": "",
     "hbciVersion": "0",
@@ -226,12 +327,12 @@
     "userID": "64769092",
     "pin": "38567" }</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -242,9 +343,9 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="str">
+      <c r="C5" s="3" t="str">
         <f aca="false">C4</f>
-        <v> {  "countryCode": "280",
+        <v>{  "countryCode": "280",
     "custID": "",
     "custID2": "",
     "hbciVersion": "0",
@@ -253,14 +354,14 @@
     "userID": "64769092",
     "pin": "38567" }</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New text, template fixed, write to xlsx does not work
</commit_message>
<xml_diff>
--- a/simpleTS/simpleTest.xlsx
+++ b/simpleTS/simpleTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Test for tranlation to js file</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>||</t>
+  </si>
+  <si>
+    <t>“dtyui”</t>
   </si>
   <si>
     <t>|</t>
@@ -157,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,10 +182,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -266,7 +265,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -327,10 +326,12 @@
     "userID": "64769092",
     "pin": "38567" }</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>

</xml_diff>